<commit_message>
Major commit, months later
</commit_message>
<xml_diff>
--- a/2023-05-25/Genealogy-Ark.xlsx
+++ b/2023-05-25/Genealogy-Ark.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="70">
   <si>
     <t>Adam</t>
   </si>
@@ -269,6 +269,21 @@
   <si>
     <t>https://en.wikipedia.org/wiki/Sena,_Yemen</t>
   </si>
+  <si>
+    <t>flood at his birth?</t>
+  </si>
+  <si>
+    <t>800 years?</t>
+  </si>
+  <si>
+    <t>150 after</t>
+  </si>
+  <si>
+    <t>https://courses.byui.edu/BOM%20Timeline/html/timeline.html</t>
+  </si>
+  <si>
+    <t>http://www.bmaf.org/articles/review_this_land_zarahemla__andersen</t>
+  </si>
 </sst>
 </file>
 
@@ -302,12 +317,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -322,9 +349,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R51"/>
+  <dimension ref="A1:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +725,7 @@
         <f>(B4-$C$14)/$C$15</f>
         <v>2.056433089928007</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <f>I4</f>
         <v>930</v>
       </c>
@@ -860,7 +889,7 @@
         <f>(B8-$C$14)/$C$15</f>
         <v>-0.75434578298761079</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <f>I8</f>
         <v>895</v>
       </c>
@@ -868,6 +897,10 @@
         <f>(D8-$E$14)/$E$15</f>
         <v>0.25265301911543869</v>
       </c>
+      <c r="F8" s="2">
+        <f>SUM(B4:B8)</f>
+        <v>960</v>
+      </c>
       <c r="G8">
         <v>65</v>
       </c>
@@ -909,6 +942,10 @@
         <f>(D9-$E$14)/$E$15</f>
         <v>0.60695481103778615</v>
       </c>
+      <c r="F9">
+        <f>SUM(B5:B9)</f>
+        <v>892</v>
+      </c>
       <c r="G9">
         <v>162</v>
       </c>
@@ -950,6 +987,10 @@
         <f>(D10-$E$14)/$E$15</f>
         <v>-2.5500327975837274</v>
       </c>
+      <c r="F10">
+        <f>SUM(B6:B10)</f>
+        <v>852</v>
+      </c>
       <c r="G10">
         <v>65</v>
       </c>
@@ -994,6 +1035,10 @@
         <f>(D11-$E$14)/$E$15</f>
         <v>0.64397141616400155</v>
       </c>
+      <c r="F11">
+        <f>SUM(B7:B11)</f>
+        <v>829</v>
+      </c>
       <c r="G11">
         <v>187</v>
       </c>
@@ -1035,6 +1080,10 @@
         <f>(D12-$E$14)/$E$15</f>
         <v>-0.37134118158362089</v>
       </c>
+      <c r="F12" s="3">
+        <f>SUM(B8:B12)</f>
+        <v>847</v>
+      </c>
       <c r="G12">
         <v>182</v>
       </c>
@@ -1054,6 +1103,12 @@
       <c r="M12">
         <f>(M11+M17)/2</f>
         <v>960</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <f>SUM(B9:B13)</f>
+        <v>682</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -1065,7 +1120,11 @@
         <f>AVERAGE(D4:D12)</f>
         <v>847.22222222222217</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14">
+        <f>SUM(B10:B14)</f>
+        <v>520</v>
+      </c>
+      <c r="G14" t="s">
         <v>24</v>
       </c>
       <c r="H14">
@@ -1090,7 +1149,11 @@
         <f>_xlfn.STDEV.S(D4:D12)</f>
         <v>189.10432159113788</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15">
+        <f>SUM(B11:B15)</f>
+        <v>355</v>
+      </c>
+      <c r="G15" t="s">
         <v>25</v>
       </c>
       <c r="H15">
@@ -1110,8 +1173,12 @@
       <c r="A16" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <f>SUM(B12:B16)</f>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1138,12 +1205,18 @@
       <c r="J17" t="s">
         <v>44</v>
       </c>
+      <c r="L17">
+        <v>165</v>
+      </c>
       <c r="M17">
         <f>I17</f>
         <v>951</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1156,8 +1229,15 @@
       <c r="G18">
         <v>103</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <f>B18</f>
+        <v>103</v>
+      </c>
+      <c r="P18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1170,8 +1250,12 @@
       <c r="G19">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <f>B19</f>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1184,8 +1268,12 @@
       <c r="G20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <f>B20</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1198,8 +1286,12 @@
       <c r="G21">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <f>B21</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1209,11 +1301,19 @@
       <c r="D22">
         <v>404</v>
       </c>
+      <c r="F22">
+        <f>SUM(B18:B22)</f>
+        <v>632</v>
+      </c>
       <c r="G22">
         <v>34</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <f>B22</f>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -1223,11 +1323,26 @@
       <c r="D23">
         <v>339</v>
       </c>
+      <c r="F23">
+        <f>F22+B23</f>
+        <v>762</v>
+      </c>
       <c r="G23">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <f>B23</f>
+        <v>130</v>
+      </c>
+      <c r="N23" t="s">
+        <v>65</v>
+      </c>
+      <c r="P23">
+        <f>SUM(L17:L22)</f>
+        <v>797</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -1237,11 +1352,19 @@
       <c r="D24">
         <v>339</v>
       </c>
+      <c r="F24">
+        <f>F23+B11</f>
+        <v>929</v>
+      </c>
       <c r="G24">
         <v>32</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <f>B24</f>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -1254,8 +1377,12 @@
       <c r="G25">
         <v>30</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <f>B25</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -1271,8 +1398,12 @@
       <c r="I26" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <f>B26</f>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -1285,8 +1416,12 @@
       <c r="G27">
         <v>70</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <f>B27</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -1297,23 +1432,38 @@
         <v>175</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>48</v>
       </c>
       <c r="B30">
         <v>86</v>
       </c>
+      <c r="E30">
+        <v>160</v>
+      </c>
+      <c r="F30">
+        <v>50</v>
+      </c>
       <c r="I30" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <f>E30*F32</f>
+        <v>4160</v>
+      </c>
+      <c r="F31">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -1322,6 +1472,10 @@
       </c>
       <c r="D32">
         <v>180</v>
+      </c>
+      <c r="F32">
+        <f>F31/F30</f>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1407,14 +1561,24 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>